<commit_message>
contactos agregados al envio de mails
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpalatam\Documents\UiPath\Consumidor Proceso de Descarga de Reportes Diarios Customer Service\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpalatam\Documents\UiPath\RPA_0014 Consumidor Proceso de Descarga de Reportes Diarios Customer Service\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="4"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -469,12 +469,6 @@
 Saludos</t>
   </si>
   <si>
-    <t>luisaaranda@berryglobal.com</t>
-  </si>
-  <si>
-    <t>luisaaranda@berryglobal.com; angelaarbelaez@berryglobal.com; sandrarosero@berryglobal.com</t>
-  </si>
-  <si>
     <t>32;{7,9};3;A:AF;Base de datos;{.|,}</t>
   </si>
   <si>
@@ -488,6 +482,12 @@
   </si>
   <si>
     <t>30;{19};3;A:AD;Base de datos;{.|,}</t>
+  </si>
+  <si>
+    <t>luisaaranda@berryglobal.com; angelaarbelaez@berryglobal.com; sandrarosero@berryglobal.com;joaquin.bracci@renewsolutions.com.br</t>
+  </si>
+  <si>
+    <t>joaquin.bracci@renewsolutions.com.br;luisaaranda@berryglobal.com;raysa.guerrero@visionyaccion.com.ar;romeu.campos@renewsolutions.com.br</t>
   </si>
 </sst>
 </file>
@@ -4394,8 +4394,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4441,7 +4441,7 @@
         <v>59</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="60.75" thickBot="1">
@@ -4458,7 +4458,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="60.75" thickBot="1">
@@ -4475,7 +4475,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="45.75" thickBot="1">
@@ -4492,7 +4492,7 @@
         <v>59</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45.75" thickBot="1">
@@ -4509,7 +4509,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105">
@@ -4526,10 +4526,10 @@
         <v>59</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="135">
+    <row r="8" spans="1:6" ht="195">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4555,7 +4555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4607,7 +4607,7 @@
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4630,7 +4630,7 @@
         <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4644,7 +4644,7 @@
         <v>113</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -4653,7 +4653,7 @@
         <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H4" t="s">
         <v>101</v>
@@ -4679,7 +4679,7 @@
         <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H5" t="s">
         <v>98</v>
@@ -4705,7 +4705,7 @@
         <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H6" t="s">
         <v>97</v>
@@ -4731,7 +4731,7 @@
         <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H7" t="s">
         <v>99</v>
@@ -4748,7 +4748,7 @@
         <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -4757,7 +4757,7 @@
         <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H8" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Agregado nuevo templatev2 para envio de mails
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -488,6 +488,20 @@
   </si>
   <si>
     <t>joaquin.bracci@renewsolutions.com.br;luisaaranda@berryglobal.com;raysa.guerrero@visionyaccion.com.ar;romeu.campos@renewsolutions.com.br</t>
+  </si>
+  <si>
+    <t>Berry Status Report Colombia</t>
+  </si>
+  <si>
+    <t>Estimados,&lt;br&gt;&lt;br&gt;
+Se adjunta 'Berry Status Report'.&lt;br&gt;&lt;br&gt;
+Saludos</t>
+  </si>
+  <si>
+    <t>gustavoconforto@berryglobal.com</t>
+  </si>
+  <si>
+    <t>maximiliano.esbiza@renewsolutions.com.br;luisaaranda@berryglobal.com;joaquin.bracci@renewsolutions.com.br</t>
   </si>
 </sst>
 </file>
@@ -612,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -662,6 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4392,10 +4407,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4427,7 +4442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="60.75" thickBot="1">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -4444,7 +4459,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="60.75" thickBot="1">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -4461,7 +4476,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" ht="60.75" thickBot="1">
+    <row r="4" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -4478,7 +4493,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="45.75" thickBot="1">
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -4495,7 +4510,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45.75" thickBot="1">
+    <row r="6" spans="1:6" ht="195.75" thickBot="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -4512,7 +4527,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105">
+    <row r="7" spans="1:6" ht="195">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -4544,6 +4559,23 @@
       </c>
       <c r="E8" s="6" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4556,7 +4588,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Agregado contactos para envio de mails de Price List Report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -498,10 +498,10 @@
 Saludos</t>
   </si>
   <si>
-    <t>gustavoconforto@berryglobal.com</t>
-  </si>
-  <si>
     <t>maximiliano.esbiza@renewsolutions.com.br;luisaaranda@berryglobal.com;joaquin.bracci@renewsolutions.com.br</t>
+  </si>
+  <si>
+    <t>EricRodrigues@berryglobal.com;KevinKruger@berryglobal.com;GustavoConforto@berryglobal.com;MurilloLima@berryglobal.com;DaniloAlmeida@berryglobal.com;mariawosiack@berryglobal.com;AndreaSoyama@berryglobal.com;VictorZanini@berryglobal.com</t>
   </si>
 </sst>
 </file>
@@ -4410,7 +4410,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4571,11 +4571,11 @@
       <c r="C9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ale panozo agregada a envio de mails
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="3"/>
+    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9456" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
 Saludos</t>
   </si>
   <si>
-    <t>maximiliano.esbiza@renewsolutions.com.br</t>
-  </si>
-  <si>
     <t>Problema al Ingresar a la Responsabilidad</t>
   </si>
   <si>
@@ -490,18 +487,21 @@
     <t>joaquin.bracci@renewsolutions.com.br;luisaaranda@berryglobal.com;raysa.guerrero@visionyaccion.com.ar;romeu.campos@renewsolutions.com.br</t>
   </si>
   <si>
-    <t>Berry Status Report Colombia</t>
+    <t>EricRodrigues@berryglobal.com;KevinKruger@berryglobal.com;GustavoConforto@berryglobal.com</t>
+  </si>
+  <si>
+    <t>COL Price List Report y Facturación</t>
   </si>
   <si>
     <t>Estimados,&lt;br&gt;&lt;br&gt;
-Se adjunta 'Berry Status Report'.&lt;br&gt;&lt;br&gt;
+Se adjuntan 'Price List Report' y 'XXARX PLANO FACTURACION EXCEL'.&lt;br&gt;&lt;br&gt;
 Saludos</t>
   </si>
   <si>
-    <t>maximiliano.esbiza@renewsolutions.com.br;luisaaranda@berryglobal.com;joaquin.bracci@renewsolutions.com.br</t>
-  </si>
-  <si>
-    <t>EricRodrigues@berryglobal.com;KevinKruger@berryglobal.com;GustavoConforto@berryglobal.com;MurilloLima@berryglobal.com;DaniloAlmeida@berryglobal.com;mariawosiack@berryglobal.com;AndreaSoyama@berryglobal.com;VictorZanini@berryglobal.com</t>
+    <t>maximiliano.esbiza@renewsolutions.com.br;alejandra.panozo@renewsolutions.com.br</t>
+  </si>
+  <si>
+    <t>alejandra.panozo@renewsolutions.com.br;maximiliano.esbiza@renewsolutions.com.br;luisaaranda@berryglobal.com;joaquin.bracci@renewsolutions.com.br</t>
   </si>
 </sst>
 </file>
@@ -999,12 +999,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1050,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -1067,26 +1067,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14.4">
       <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1095,7 +1095,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -1104,7 +1104,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1115,12 +1115,12 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -1131,10 +1131,10 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2135,12 +2135,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2177,7 +2177,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2302,7 +2302,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3299,12 +3299,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3345,52 +3345,52 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3398,10 +3398,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
         <v>124</v>
-      </c>
-      <c r="C6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4410,19 +4410,19 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="35.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.44140625" style="3"/>
+    <col min="2" max="2" width="35.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="63.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="173.4" thickBot="1">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -4452,116 +4452,116 @@
       <c r="C2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>59</v>
+      <c r="D2" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="173.4" thickBot="1">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>59</v>
+        <v>125</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
+    <row r="4" spans="1:6" s="6" customFormat="1" ht="173.4" thickBot="1">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>59</v>
+      <c r="D4" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="195.75" thickBot="1">
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="173.4" thickBot="1">
       <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>59</v>
+        <v>128</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="195.75" thickBot="1">
+    <row r="6" spans="1:6" ht="173.4" thickBot="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>59</v>
+      <c r="D6" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="195">
+    <row r="7" spans="1:6" ht="172.8">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>130</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="195">
+    <row r="8" spans="1:6" ht="172.8">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>59</v>
+      <c r="D8" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="57.6">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -4572,10 +4572,10 @@
         <v>147</v>
       </c>
       <c r="D9" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -4588,211 +4588,211 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
         <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
         <v>133</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>115</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -4809,68 +4809,68 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>44</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="255">
+    <row r="2" spans="1:8" ht="230.4">
       <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>